<commit_message>
Enviado avance tarea 7,Article
</commit_message>
<xml_diff>
--- a/src/test/resources/data/testData.xlsx
+++ b/src/test/resources/data/testData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a877d6f23a3de7d5/Lapto/Cursos/Selenium 4/ClasesCarlos/Sesion_X/Selenium_Tarea-7/src/test/resources/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="64" documentId="13_ncr:1_{B664314F-848F-7946-9835-BC8806769DE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B532C8CE-C584-467A-B901-AE39F7875037}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="13_ncr:1_{1478D1C1-88AE-4E2F-BD02-DE28CDE521A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BBE23FF6-6416-4E0E-AE0D-352DE95FB1D4}"/>
   <bookViews>
-    <workbookView xWindow="2670" yWindow="0" windowWidth="15405" windowHeight="10920" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="errorMessages" sheetId="5" r:id="rId1"/>
@@ -58,15 +58,9 @@
     <t>password</t>
   </si>
   <si>
-    <t>u1000@correo.com</t>
-  </si>
-  <si>
     <t>email</t>
   </si>
   <si>
-    <t>u1000</t>
-  </si>
-  <si>
     <t>noel</t>
   </si>
   <si>
@@ -83,6 +77,12 @@
   </si>
   <si>
     <t>a583up48pq</t>
+  </si>
+  <si>
+    <t>u11000</t>
+  </si>
+  <si>
+    <t>u11000@correo.com</t>
   </si>
 </sst>
 </file>
@@ -458,7 +458,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -477,7 +477,7 @@
         <v>8</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D1" s="7" t="s">
         <v>9</v>
@@ -488,10 +488,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="D2" s="5">
         <v>123</v>
@@ -502,13 +502,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="5" t="s">
         <v>13</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -516,13 +516,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="5" t="s">
         <v>16</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:4">

</xml_diff>